<commit_message>
added data driven concept using Excel
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/registrationdata.xlsx
+++ b/src/test/resources/testdata/registrationdata.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>firstname</t>
   </si>
@@ -19,9 +19,6 @@
     <t>lastname</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
     <t>phone</t>
   </si>
   <si>
@@ -34,13 +31,13 @@
     <t>gender</t>
   </si>
   <si>
-    <t>testuser1</t>
-  </si>
-  <si>
-    <t>lastname1</t>
-  </si>
-  <si>
-    <t>testlast1@gmail.com</t>
+    <t>testuser5</t>
+  </si>
+  <si>
+    <t>lastname5</t>
+  </si>
+  <si>
+    <t>1234567898</t>
   </si>
   <si>
     <t>Selenium@123</t>
@@ -52,13 +49,13 @@
     <t>male</t>
   </si>
   <si>
-    <t>testuser2</t>
-  </si>
-  <si>
-    <t>lastname2</t>
-  </si>
-  <si>
-    <t>testlast2@gmail.com</t>
+    <t>testuser6</t>
+  </si>
+  <si>
+    <t>lastname6</t>
+  </si>
+  <si>
+    <t>2234567898</t>
   </si>
   <si>
     <t>Selenium@124</t>
@@ -70,13 +67,13 @@
     <t>female</t>
   </si>
   <si>
-    <t>testuser3</t>
-  </si>
-  <si>
-    <t>lastname3</t>
-  </si>
-  <si>
-    <t>testlast3@gmail.com</t>
+    <t>testuser7</t>
+  </si>
+  <si>
+    <t>lastname7</t>
+  </si>
+  <si>
+    <t>3123456789</t>
   </si>
   <si>
     <t>Selenium@125</t>
@@ -85,13 +82,13 @@
     <t>Engineer</t>
   </si>
   <si>
-    <t>testuser4</t>
-  </si>
-  <si>
-    <t>lastname4</t>
-  </si>
-  <si>
-    <t>testlast4@gmail.com</t>
+    <t>testuser8</t>
+  </si>
+  <si>
+    <t>lastname8</t>
+  </si>
+  <si>
+    <t>4234567898</t>
   </si>
   <si>
     <t>Selenium@126</t>
@@ -151,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -159,6 +156,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf quotePrefix="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -376,9 +376,6 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="3" max="3" width="16.5"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -399,100 +396,85 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1.234567898E9</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="D3" s="2">
-        <v>2.234567898E9</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="D4" s="2">
-        <v>3.123456789E9</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="D5" s="2">
-        <v>4.234567898E9</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>